<commit_message>
Parte 2 punto 1
</commit_message>
<xml_diff>
--- a/Credito/Credito-parte1.xlsx
+++ b/Credito/Credito-parte1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mippolimi-my.sharepoint.com/personal/giorgio_cappello_gsom_polimi_it/Documents/Desktop/Valutazione Prodotti/Progetto/Anno corrente/ProgettoValutazioneProdotti/Credito/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="681" documentId="8_{63744DCE-6C42-41B8-B74E-D1CE19CF747E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F748345C-331D-49B9-80DE-0E4A0258D968}"/>
+  <xr:revisionPtr revIDLastSave="682" documentId="8_{63744DCE-6C42-41B8-B74E-D1CE19CF747E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3252FD87-8F8D-4551-9BC8-608E71BFB724}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{07B42D37-A8E8-4F59-80DE-7E765F4C4A6C}"/>
+    <workbookView minimized="1" xWindow="5115" yWindow="1965" windowWidth="15375" windowHeight="7875" xr2:uid="{07B42D37-A8E8-4F59-80DE-7E765F4C4A6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Gruppo 1" sheetId="1" r:id="rId1"/>
@@ -604,6 +604,12 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -618,12 +624,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2148,7 +2148,7 @@
   <dimension ref="A1:XFD1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2170,22 +2170,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="65"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="67"/>
     </row>
     <row r="3" spans="1:12" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="67"/>
-      <c r="D3" s="68" t="s">
+      <c r="B3" s="69"/>
+      <c r="D3" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="69">
+      <c r="E3" s="64">
         <v>2.5486258974545904E-2</v>
       </c>
     </row>
@@ -2476,7 +2476,7 @@
         <v>0.24336144767736889</v>
       </c>
       <c r="F14" s="51">
-        <f t="shared" ref="F11:F14" si="2">EXP(-E14)</f>
+        <f t="shared" ref="F14" si="2">EXP(-E14)</f>
         <v>0.78398809187865526</v>
       </c>
       <c r="G14" s="48">

</xml_diff>